<commit_message>
Add a logger and remove setup sheets
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,29 +13,25 @@
     <sheet name="Rooms" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Speakers" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Talks" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="talkTypeOfTimeslot_setup" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="talkTypeOfTimeslot_timeslotWithMatchingTalkType" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="talkTypeOfTimeslot_timeslotWithNonMatchingTalkType" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="talkHasUnavailableRoom_setup" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="talkHasUnavailableRoom_talkWithAvailableRoom" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="talkHasUnavailableRoom_talkWithUnavailableRoom" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="talkHasUnavailableRoom_talkWithAvailableRoom_2" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="talkHasUnavailableRoom_talkWithUnavailableRoom_2" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="roomConflict_setup" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="roomConflict_talksInSameRoomWithoutOverlappingTimeslots" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="roomConflict_talksInSameRoomWithOverlappingTimeslots" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="roomConflict_talksInDifferentRoomsWithOverlappingTimeslots" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="talkWithUnavailableSpeaker_setup" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableSpeaker" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableSpeaker_2" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableTwoSpeakers" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableTwoSpeakers_2" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="talkWithUnavailableSpeaker_talkWithOneOrMoreUnavailableSpeaker" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="talkWithUnavailableSpeaker_talkWithOneOrMoreUnavailableSpeaker_2" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="talkWithUnavailableSpeaker_talkWithOneOrMoreUnavailableSpeaker_3" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="speakerConflict_setup" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="speakerConflict_speakerHasNoConflictingTimeslots" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="speakerConflict_speakerHasConflictingTimeslots" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="talkTypeOfTimeslot_timeslotWithMatchingTalkType" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="talkTypeOfTimeslot_timeslotWithNonMatchingTalkType" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="talkHasUnavailableRoom_setup" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="talkHasUnavailableRoom_talkWithAvailableRoom" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="talkHasUnavailableRoom_talkWithUnavailableRoom" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="talkHasUnavailableRoom_talkWithAvailableRoom_2" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="talkHasUnavailableRoom_talkWithUnavailableRoom_2" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="roomConflict_talksInSameRoomWithoutOverlappingTimeslots" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="roomConflict_talksInSameRoomWithOverlappingTimeslots" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="roomConflict_talksInDifferentRoomsWithOverlappingTimeslots" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableSpeaker" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableSpeaker_2" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableTwoSpeakers" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="talkWithUnavailableSpeaker_talkWithoutUnavailableTwoSpeakers_2" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="talkWithUnavailableSpeaker_talkWithOneOrMoreUnavailableSpeaker" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="talkWithUnavailableSpeaker_talkWithOneOrMoreUnavailableSpeaker_2" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="talkWithUnavailableSpeaker_talkWithOneOrMoreUnavailableSpeaker_3" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="speakerConflict_speakerHasNoConflictingTimeslots" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="speakerConflict_speakerHasConflictingTimeslots" sheetId="24" state="visible" r:id="rId25"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -47,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="140">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -850,7 +846,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="A20:C20 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1223,7 +1219,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="1" sqref="A20:C20 A10"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1275,7 +1271,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1345,9 +1341,6 @@
       <c r="A7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
@@ -1364,7 +1357,6 @@
       <c r="A8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -1381,7 +1373,9 @@
       <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="C9" s="11"/>
       <c r="D9" s="4"/>
       <c r="E9" s="11"/>
@@ -1445,7 +1439,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="1" sqref="A20:C20 A10"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1497,7 +1491,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1583,6 +1577,9 @@
       <c r="A8" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -1599,9 +1596,7 @@
       <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="11"/>
       <c r="D9" s="4"/>
       <c r="E9" s="11"/>
@@ -1665,7 +1660,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="1" sqref="A20:C20 A10"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1717,7 +1712,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1803,9 +1798,6 @@
       <c r="A8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -1822,7 +1814,6 @@
       <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="4"/>
       <c r="C9" s="11"/>
       <c r="D9" s="4"/>
       <c r="E9" s="11"/>
@@ -1839,7 +1830,9 @@
       <c r="A10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1879,14 +1872,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="1" sqref="A20:C20 A10"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1920,7 +1913,7 @@
         <v>133</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1938,7 +1931,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1969,10 +1962,10 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="11"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -1990,10 +1983,12 @@
       <c r="B6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -2005,11 +2000,16 @@
       <c r="M6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>81</v>
+      <c r="A7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2021,9 +2021,10 @@
       <c r="M7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="A8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -2036,41 +2037,8 @@
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2078,9 +2046,8 @@
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F9:H9"/>
+  <mergeCells count="1">
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2105,7 +2072,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="1" sqref="A20:C20 B5"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2157,7 +2124,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2229,9 +2196,12 @@
       <c r="A7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2294,7 +2264,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="1" sqref="A20:C20 B5"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2418,12 +2388,8 @@
       <c r="A7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
@@ -2440,7 +2406,9 @@
         <v>86</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="C8" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
@@ -2480,14 +2448,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="1" sqref="A20:C20 B5"/>
+      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2520,8 +2488,8 @@
       <c r="A2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>38</v>
+      <c r="B2" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2539,7 +2507,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2570,10 +2538,10 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -2591,12 +2559,10 @@
       <c r="B6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -2609,14 +2575,13 @@
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>120</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2627,23 +2592,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2654,7 +2603,7 @@
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2672,14 +2621,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="1" sqref="A20:C20 B5"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2712,8 +2661,8 @@
       <c r="A2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>38</v>
+      <c r="B2" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2762,10 +2711,10 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -2783,12 +2732,10 @@
       <c r="B6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -2801,11 +2748,12 @@
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>119</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2816,25 +2764,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2845,7 +2775,7 @@
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2870,7 +2800,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="1" sqref="A20:C20 B5"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2992,8 +2922,9 @@
       <c r="A7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
@@ -3041,7 +2972,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="1" sqref="A20:C20 B7"/>
+      <selection pane="bottomRight" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3163,10 +3094,10 @@
       <c r="A7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="6"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
@@ -3213,7 +3144,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" activeCellId="1" sqref="A20:C20 A19"/>
+      <selection pane="bottomRight" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3477,7 +3408,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="1" sqref="A20:C20 B8"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3529,7 +3460,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3599,8 +3530,8 @@
       <c r="A7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>121</v>
+      <c r="B7" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
@@ -3649,7 +3580,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="1" sqref="A20:C20 B8"/>
+      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3701,7 +3632,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3772,7 +3703,7 @@
         <v>87</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
@@ -3821,7 +3752,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C7" activeCellId="1" sqref="A20:C20 C7"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3873,7 +3804,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3943,9 +3874,8 @@
       <c r="A7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>122</v>
+      <c r="B7" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
@@ -3994,7 +3924,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="1" sqref="A20:C20 B4"/>
+      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4028,7 +3958,7 @@
         <v>133</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -4046,7 +3976,7 @@
         <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -4077,10 +4007,10 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="11"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -4099,9 +4029,11 @@
         <v>77</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4113,13 +4045,16 @@
       <c r="M6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="7"/>
+      <c r="A7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -4141,7 +4076,7 @@
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4166,701 +4101,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="1" sqref="A20:C20 B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:C5"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M8"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="1" sqref="A20:C20 B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:C5"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M8"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="1" sqref="A20:C20 B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:D5"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M8"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C8" activeCellId="1" sqref="A20:C20 C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:D5"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M8"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="1" sqref="A20:C20 A7"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5035,7 +4276,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P1" activeCellId="1" sqref="A20:C20 P1"/>
+      <selection pane="bottomRight" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5396,7 +4637,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A11" activeCellId="1" sqref="A20:C20 A11"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5757,12 +4998,12 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A20" activeCellId="0" sqref="A20:C20"/>
+      <selection pane="bottomRight" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7833,12 +7074,12 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="1" sqref="A20:C20 B5"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7960,7 +7201,9 @@
       <c r="A7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="13" t="s">
+        <v>115</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
@@ -8009,7 +7252,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="1" sqref="A20:C20 B5"/>
+      <selection pane="bottomRight" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8134,7 +7377,9 @@
       <c r="B7" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
@@ -8175,14 +7420,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C7" activeCellId="1" sqref="A20:C20 C7"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8215,8 +7460,8 @@
       <c r="A2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>33</v>
+      <c r="B2" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -8265,7 +7510,7 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="11"/>
@@ -8302,14 +7547,10 @@
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>116</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
@@ -8321,9 +7562,57 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8331,8 +7620,9 @@
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -8357,7 +7647,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="1" sqref="A20:C20 A10"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8479,7 +7769,9 @@
       <c r="A7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>

</xml_diff>

<commit_message>
Remove unnecessary fields and fix indentations
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="117">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -265,9 +265,6 @@
   </si>
   <si>
     <t xml:space="preserve">unavailableRoom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri 2018-01-05</t>
   </si>
   <si>
     <t xml:space="preserve">Required timeslot tags</t>
@@ -518,11 +515,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1015,11 +1012,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1032,10 +1029,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1050,7 +1047,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>38</v>
@@ -1068,10 +1065,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1118,7 +1115,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -1143,20 +1140,20 @@
       <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -1192,11 +1189,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1209,10 +1206,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1227,7 +1224,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>38</v>
@@ -1245,10 +1242,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1295,7 +1292,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -1320,19 +1317,19 @@
       <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -1368,11 +1365,11 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1385,10 +1382,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1403,7 +1400,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>38</v>
@@ -1421,10 +1418,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1471,7 +1468,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -1497,15 +1494,15 @@
         <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -1513,18 +1510,18 @@
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="4"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
@@ -1559,11 +1556,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1576,10 +1573,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1594,7 +1591,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>40</v>
@@ -1612,10 +1609,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1662,7 +1659,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -1688,16 +1685,16 @@
         <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -1733,11 +1730,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1750,10 +1747,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1768,7 +1765,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>40</v>
@@ -1786,10 +1783,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1836,7 +1833,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -1863,16 +1860,16 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -1908,11 +1905,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1925,10 +1922,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1943,7 +1940,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>40</v>
@@ -1961,10 +1958,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2011,7 +2008,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -2037,16 +2034,16 @@
         <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -2082,11 +2079,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2099,10 +2096,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2115,9 +2112,9 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>40</v>
@@ -2135,10 +2132,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2185,7 +2182,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -2211,16 +2208,16 @@
         <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -2256,11 +2253,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2273,10 +2270,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2291,7 +2288,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>42</v>
@@ -2309,10 +2306,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2359,7 +2356,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -2385,19 +2382,19 @@
         <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -2433,11 +2430,11 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2450,10 +2447,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2468,7 +2465,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>42</v>
@@ -2486,10 +2483,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -2562,15 +2559,15 @@
         <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -2578,18 +2575,18 @@
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="4"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
@@ -2622,12 +2619,12 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2733,14 +2730,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2808,25 +2805,17 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2854,7 +2843,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2888,9 +2877,7 @@
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
@@ -2899,28 +2886,28 @@
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>70</v>
@@ -2931,19 +2918,13 @@
       <c r="L2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -2954,15 +2935,15 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2973,15 +2954,15 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2992,15 +2973,15 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -3039,12 +3020,12 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3076,64 +3057,64 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>57</v>
@@ -3142,19 +3123,19 @@
         <v>58</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3180,14 +3161,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -3211,15 +3192,23 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -3236,16 +3225,16 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3269,16 +3258,16 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -3326,39 +3315,6 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
@@ -4824,11 +4780,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4841,10 +4797,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4859,7 +4815,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -4877,10 +4833,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -4927,7 +4883,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -4953,17 +4909,17 @@
         <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -4999,11 +4955,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5016,10 +4972,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5034,7 +4990,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -5052,10 +5008,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5102,7 +5058,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -5124,21 +5080,21 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -5174,11 +5130,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5191,10 +5147,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5209,7 +5165,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>36</v>
@@ -5227,10 +5183,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5277,7 +5233,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -5299,21 +5255,21 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
@@ -5349,11 +5305,11 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5366,10 +5322,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5384,7 +5340,7 @@
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>36</v>
@@ -5402,10 +5358,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5452,7 +5408,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -5474,20 +5430,20 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>102</v>
+      <c r="C7" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>

</xml_diff>

<commit_message>
Convert into parameterized test
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -398,7 +398,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -428,20 +428,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -498,7 +488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -515,23 +505,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -543,19 +521,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1031,14 +1001,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1049,14 +1019,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1067,14 +1037,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1083,13 +1053,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1103,15 +1073,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1120,42 +1090,42 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1208,14 +1178,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1226,14 +1196,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1244,14 +1214,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1260,13 +1230,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1280,15 +1250,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1297,41 +1267,41 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1384,14 +1354,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1402,14 +1372,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1420,14 +1390,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1436,13 +1406,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1456,15 +1426,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1473,21 +1443,21 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -1496,34 +1466,34 @@
       <c r="B7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1575,14 +1545,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1593,14 +1563,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1611,14 +1581,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1627,13 +1597,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1647,15 +1617,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1664,21 +1634,21 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -1687,16 +1657,16 @@
       <c r="C7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1749,14 +1719,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1767,14 +1737,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1785,14 +1755,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1801,13 +1771,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1821,15 +1791,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1838,21 +1808,21 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -1862,16 +1832,16 @@
       <c r="C7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1924,14 +1894,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1942,14 +1912,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1960,14 +1930,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1976,13 +1946,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1996,15 +1966,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -2013,21 +1983,21 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -2036,16 +2006,16 @@
       <c r="B7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2098,14 +2068,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -2116,14 +2086,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2134,14 +2104,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -2150,13 +2120,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2170,15 +2140,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -2187,21 +2157,21 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -2210,16 +2180,16 @@
       <c r="B7" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2272,14 +2242,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -2290,14 +2260,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2308,14 +2278,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -2324,13 +2294,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2344,15 +2314,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -2367,15 +2337,15 @@
       <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -2384,19 +2354,19 @@
       <c r="B7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2449,14 +2419,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -2467,14 +2437,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2485,14 +2455,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -2501,13 +2471,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2521,15 +2491,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -2544,15 +2514,15 @@
       <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -2561,34 +2531,34 @@
       <c r="B7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2619,7 +2589,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -2806,16 +2776,16 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2912,10 +2882,10 @@
       <c r="J2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="1" t="s">
         <v>72</v>
       </c>
       <c r="M2" s="1"/>
@@ -2926,77 +2896,77 @@
       <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3127,7 +3097,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="2"/>
@@ -3153,7 +3123,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="9"/>
+      <c r="S2" s="6"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -3186,7 +3156,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="9"/>
+      <c r="S3" s="6"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
@@ -3219,7 +3189,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="9"/>
+      <c r="S4" s="6"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
@@ -3252,7 +3222,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="9"/>
+      <c r="S5" s="6"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
@@ -3285,7 +3255,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="9"/>
+      <c r="S6" s="6"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
@@ -3310,7 +3280,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="9"/>
+      <c r="S7" s="6"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
@@ -3335,7 +3305,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="9"/>
+      <c r="S9" s="6"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
@@ -3360,7 +3330,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="9"/>
+      <c r="S10" s="6"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
@@ -3385,7 +3355,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="9"/>
+      <c r="S11" s="6"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
@@ -3410,7 +3380,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="9"/>
+      <c r="S12" s="6"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
@@ -3435,7 +3405,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="9"/>
+      <c r="S13" s="6"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
@@ -3460,7 +3430,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="9"/>
+      <c r="S14" s="6"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
@@ -3485,7 +3455,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="9"/>
+      <c r="S15" s="6"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
@@ -3510,7 +3480,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="9"/>
+      <c r="S16" s="6"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
@@ -3535,7 +3505,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="9"/>
+      <c r="S17" s="6"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
@@ -3560,7 +3530,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="9"/>
+      <c r="S18" s="6"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
@@ -3585,7 +3555,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="9"/>
+      <c r="S19" s="6"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
@@ -3610,7 +3580,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="9"/>
+      <c r="S20" s="6"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
@@ -3635,7 +3605,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="9"/>
+      <c r="S21" s="6"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
@@ -3660,7 +3630,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="9"/>
+      <c r="S22" s="6"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
@@ -3685,7 +3655,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="9"/>
+      <c r="S23" s="6"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
@@ -3710,7 +3680,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="9"/>
+      <c r="S24" s="6"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
@@ -3735,7 +3705,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="9"/>
+      <c r="S25" s="6"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
@@ -3760,7 +3730,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="9"/>
+      <c r="S26" s="6"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
@@ -3785,7 +3755,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="9"/>
+      <c r="S27" s="6"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
@@ -3810,7 +3780,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="9"/>
+      <c r="S28" s="6"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
@@ -3835,7 +3805,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="9"/>
+      <c r="S29" s="6"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
@@ -3860,7 +3830,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="9"/>
+      <c r="S30" s="6"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
@@ -3885,7 +3855,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="9"/>
+      <c r="S31" s="6"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
@@ -3910,7 +3880,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="9"/>
+      <c r="S32" s="6"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
@@ -3935,7 +3905,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-      <c r="S33" s="9"/>
+      <c r="S33" s="6"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
@@ -3960,7 +3930,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-      <c r="S34" s="9"/>
+      <c r="S34" s="6"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
@@ -3985,7 +3955,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-      <c r="S35" s="9"/>
+      <c r="S35" s="6"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
@@ -4010,7 +3980,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-      <c r="S36" s="9"/>
+      <c r="S36" s="6"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
@@ -4035,7 +4005,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
-      <c r="S37" s="9"/>
+      <c r="S37" s="6"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
@@ -4060,7 +4030,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
-      <c r="S38" s="9"/>
+      <c r="S38" s="6"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
@@ -4085,7 +4055,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
-      <c r="S39" s="9"/>
+      <c r="S39" s="6"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
@@ -4110,7 +4080,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
-      <c r="S40" s="9"/>
+      <c r="S40" s="6"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
@@ -4135,7 +4105,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
-      <c r="S41" s="9"/>
+      <c r="S41" s="6"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
@@ -4160,7 +4130,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
-      <c r="S42" s="9"/>
+      <c r="S42" s="6"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
@@ -4185,7 +4155,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-      <c r="S43" s="9"/>
+      <c r="S43" s="6"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
@@ -4210,7 +4180,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
-      <c r="S44" s="9"/>
+      <c r="S44" s="6"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
@@ -4235,7 +4205,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-      <c r="S45" s="9"/>
+      <c r="S45" s="6"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
@@ -4260,7 +4230,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-      <c r="S46" s="9"/>
+      <c r="S46" s="6"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
@@ -4285,7 +4255,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
-      <c r="S47" s="9"/>
+      <c r="S47" s="6"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
@@ -4310,7 +4280,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
-      <c r="S48" s="9"/>
+      <c r="S48" s="6"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
@@ -4335,7 +4305,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
-      <c r="S49" s="9"/>
+      <c r="S49" s="6"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
@@ -4360,7 +4330,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
-      <c r="S50" s="9"/>
+      <c r="S50" s="6"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
@@ -4385,7 +4355,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
-      <c r="S51" s="9"/>
+      <c r="S51" s="6"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
@@ -4410,7 +4380,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
-      <c r="S52" s="9"/>
+      <c r="S52" s="6"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
@@ -4435,7 +4405,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
-      <c r="S53" s="9"/>
+      <c r="S53" s="6"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
@@ -4460,7 +4430,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
-      <c r="S54" s="9"/>
+      <c r="S54" s="6"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
@@ -4485,7 +4455,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="9"/>
+      <c r="S55" s="6"/>
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
@@ -4510,7 +4480,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
-      <c r="S56" s="9"/>
+      <c r="S56" s="6"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
@@ -4535,7 +4505,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
-      <c r="S57" s="9"/>
+      <c r="S57" s="6"/>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
@@ -4560,7 +4530,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
-      <c r="S58" s="9"/>
+      <c r="S58" s="6"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
@@ -4585,7 +4555,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
-      <c r="S59" s="9"/>
+      <c r="S59" s="6"/>
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
@@ -4610,7 +4580,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
-      <c r="S60" s="9"/>
+      <c r="S60" s="6"/>
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
@@ -4635,7 +4605,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
-      <c r="S61" s="9"/>
+      <c r="S61" s="6"/>
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
@@ -4660,7 +4630,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
-      <c r="S62" s="9"/>
+      <c r="S62" s="6"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
@@ -4685,7 +4655,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
-      <c r="S63" s="9"/>
+      <c r="S63" s="6"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
@@ -4710,7 +4680,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
-      <c r="S64" s="9"/>
+      <c r="S64" s="6"/>
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
@@ -4735,7 +4705,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
-      <c r="S65" s="10"/>
+      <c r="S65" s="7"/>
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
@@ -4799,14 +4769,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -4817,14 +4787,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4835,14 +4805,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -4851,13 +4821,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -4871,15 +4841,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -4888,21 +4858,21 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -4911,17 +4881,17 @@
       <c r="B7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4954,12 +4924,12 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4974,14 +4944,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -4992,14 +4962,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5010,14 +4980,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -5026,13 +4996,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -5046,15 +5016,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -5063,40 +5033,40 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5149,14 +5119,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -5167,14 +5137,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5185,14 +5155,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -5201,13 +5171,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -5221,15 +5191,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -5238,40 +5208,40 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5324,14 +5294,14 @@
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -5342,14 +5312,14 @@
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5360,14 +5330,14 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -5376,13 +5346,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -5396,15 +5366,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -5413,39 +5383,39 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add testSheetName as the name of unit test
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Rooms" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Speakers" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Talks" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="talkTypeOfTimeslot_timeslotWithMatchingTalkType" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="talkTypeOfTimeslot_timeslotWithNonMatchingTalkType" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Talk type of timeslot 1" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Talk type of timeslot 2" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="talkHasUnavailableRoom_talkWithAvailableRoom" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="talkHasUnavailableRoom_talkWithUnavailableRoom" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="roomConflict_talksInSameRoomWithoutOverlappingTimeslots" sheetId="10" state="visible" r:id="rId11"/>
@@ -1530,7 +1530,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4747,14 +4747,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4902,6 +4902,7 @@
     <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:D5"/>
@@ -4929,7 +4930,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5104,7 +5105,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5279,7 +5280,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Set soft constraints' weights to 1
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -684,12 +684,12 @@
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -724,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -735,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -757,7 +757,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -779,7 +779,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -790,7 +790,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -801,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>20</v>
@@ -812,7 +812,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>22</v>
@@ -823,7 +823,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
@@ -834,7 +834,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -845,7 +845,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>24</v>
@@ -856,7 +856,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -867,7 +867,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>30</v>
@@ -878,7 +878,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -889,7 +889,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -2424,7 +2424,7 @@
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>

</xml_diff>

<commit_message>
Fix conference name in test file
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -42,7 +42,7 @@
     <t xml:space="preserve">Conference name</t>
   </si>
   <si>
-    <t xml:space="preserve">JayFocus 2023</t>
+    <t xml:space="preserve">Junit test</t>
   </si>
   <si>
     <t xml:space="preserve">Constraint</t>
@@ -689,7 +689,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -700,7 +700,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add test cases for Talk prerequisite talks constraint
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,6 +31,14 @@
     <sheet name="Talk mutually-exclusive-talks tag 3" sheetId="21" state="visible" r:id="rId22"/>
     <sheet name="Talk mutually-exclusive-talks tag 4" sheetId="22" state="visible" r:id="rId23"/>
     <sheet name="Talk mutually-exclusive-talks tag 5" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Talk prerequisite talks" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="Talk prerequisite talks 2" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Talk prerequisite talks 3" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="Talk prerequisite talks 4" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="Talk prerequisite talks 5" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="Talk prerequisite talks 6" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="Talk prerequisite talks 7" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="Talk prerequisite talks 8" sheetId="31" state="visible" r:id="rId32"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -42,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="153">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -266,6 +274,9 @@
     <t xml:space="preserve">11:00</t>
   </si>
   <si>
+    <t xml:space="preserve">12:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
@@ -407,6 +418,43 @@
     <t xml:space="preserve">RedHat talk 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Talk with Normal talk as prerequisite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talk with Normal talk and Normal talk 2 as prerequisites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal talk, Normal talk2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Talk with (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Talk with Normal talk as prerequisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) as a prerequisite</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Constraint package</t>
   </si>
   <si>
@@ -477,6 +525,15 @@
   </si>
   <si>
     <t xml:space="preserve">-3hard/0soft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talk scheduled after its prerequisites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:00-12:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talk scheduled before its prerequisites</t>
   </si>
 </sst>
 </file>
@@ -487,7 +544,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -515,6 +572,11 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -634,7 +696,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,11 +720,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -755,7 +817,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1176,10 +1238,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1194,7 +1256,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>39</v>
@@ -1215,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1230,10 +1292,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1280,16 +1342,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1303,14 +1365,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -1371,10 +1433,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1389,7 +1451,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>39</v>
@@ -1410,7 +1472,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1425,10 +1487,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1475,16 +1537,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1498,13 +1560,13 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -1565,10 +1627,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1583,7 +1645,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>39</v>
@@ -1604,7 +1666,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1619,10 +1681,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1669,16 +1731,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1692,10 +1754,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -1709,11 +1771,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -1774,10 +1836,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1792,7 +1854,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -1813,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1828,10 +1890,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1878,16 +1940,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1901,10 +1963,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -1966,10 +2028,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1984,7 +2046,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2005,7 +2067,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2020,10 +2082,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2070,16 +2132,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2093,11 +2155,11 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -2159,10 +2221,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2177,7 +2239,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2198,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2213,10 +2275,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2263,16 +2325,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2286,10 +2348,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -2351,10 +2413,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2369,7 +2431,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2390,7 +2452,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2405,10 +2467,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2455,16 +2517,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2478,10 +2540,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -2543,10 +2605,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2561,7 +2623,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2582,7 +2644,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2597,10 +2659,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2647,16 +2709,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2670,14 +2732,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -2738,10 +2800,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2756,7 +2818,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>43</v>
@@ -2777,7 +2839,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2792,10 +2854,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2842,16 +2904,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2865,10 +2927,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -2882,11 +2944,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -2947,10 +3009,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2965,7 +3027,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -2986,7 +3048,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3001,10 +3063,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3051,16 +3113,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -3074,13 +3136,13 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -3127,7 +3189,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3201,7 +3263,20 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3254,10 +3329,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3272,7 +3347,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3293,7 +3368,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3308,10 +3383,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3358,16 +3433,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -3381,10 +3456,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="15"/>
@@ -3399,10 +3474,10 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -3464,10 +3539,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3482,7 +3557,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3503,7 +3578,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3518,10 +3593,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3568,16 +3643,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -3591,10 +3666,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -3610,11 +3685,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -3675,10 +3750,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3693,7 +3768,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3714,7 +3789,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3729,10 +3804,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3779,16 +3854,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -3802,14 +3877,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -3823,11 +3898,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -3870,7 +3945,7 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -3888,10 +3963,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3906,7 +3981,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3927,7 +4002,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3942,10 +4017,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3992,16 +4067,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -4015,10 +4090,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -4034,11 +4109,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -4053,12 +4128,1216 @@
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
+      <c r="B9" s="15"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="E8" activeCellId="0" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4118,7 +5397,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>64</v>
@@ -4127,18 +5406,18 @@
         <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>69</v>
@@ -4150,7 +5429,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>69</v>
@@ -4162,7 +5441,7 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>69</v>
@@ -4174,7 +5453,7 @@
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>69</v>
@@ -4187,6 +5466,396 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="8" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="8" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4250,40 +5919,40 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -4291,7 +5960,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4310,7 +5979,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4329,7 +5998,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -4348,7 +6017,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4388,11 +6057,11 @@
   <dimension ref="A1:Y65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4426,70 +6095,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>62</v>
@@ -4498,19 +6167,19 @@
         <v>63</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -4536,14 +6205,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4569,14 +6238,14 @@
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4602,14 +6271,14 @@
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4635,14 +6304,14 @@
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -4668,7 +6337,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -4690,7 +6359,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="6"/>
@@ -4701,18 +6370,18 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>69</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -4734,7 +6403,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="6"/>
@@ -4743,10 +6412,14 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4763,17 +6436,23 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
+      <c r="T10" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="U10" s="6"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4790,17 +6469,23 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
+      <c r="T11" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="U11" s="6"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
+    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -4817,7 +6502,9 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
+      <c r="T12" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="U12" s="6"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
@@ -6292,10 +7979,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -6310,7 +7997,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>33</v>
@@ -6331,7 +8018,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -6346,10 +8033,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -6396,16 +8083,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -6419,10 +8106,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -6485,10 +8172,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -6503,7 +8190,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>33</v>
@@ -6524,7 +8211,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -6539,10 +8226,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -6589,16 +8276,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -6612,11 +8299,11 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
@@ -6678,10 +8365,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -6696,7 +8383,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>37</v>
@@ -6717,7 +8404,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -6732,10 +8419,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -6782,16 +8469,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -6805,10 +8492,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -6871,10 +8558,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -6889,7 +8576,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>37</v>
@@ -6910,7 +8597,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -6925,10 +8612,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -6975,16 +8662,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -6998,10 +8685,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>

</xml_diff>

<commit_message>
Implement Talk mutually-exclusive-talks tag constraint and fix typos in test file
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="30"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="153">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -289,6 +289,9 @@
     <t xml:space="preserve">10:00-11:00</t>
   </si>
   <si>
+    <t xml:space="preserve">11:00-12:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Normal room</t>
   </si>
   <si>
@@ -424,7 +427,7 @@
     <t xml:space="preserve">Talk with Normal talk and Normal talk 2 as prerequisites</t>
   </si>
   <si>
-    <t xml:space="preserve">Normal talk, Normal talk2</t>
+    <t xml:space="preserve">Normal talk, Normal talk 2</t>
   </si>
   <si>
     <r>
@@ -528,9 +531,6 @@
   </si>
   <si>
     <t xml:space="preserve">Talk scheduled after its prerequisites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11:00-12:00</t>
   </si>
   <si>
     <t xml:space="preserve">Talk scheduled before its prerequisites</t>
@@ -1238,10 +1238,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>39</v>
@@ -1277,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -1365,14 +1365,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -1433,10 +1433,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>39</v>
@@ -1472,7 +1472,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1487,10 +1487,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -1627,10 +1627,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>39</v>
@@ -1666,7 +1666,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -1754,10 +1754,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -1771,11 +1771,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -1836,10 +1836,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -1875,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1890,10 +1890,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -2028,10 +2028,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2067,7 +2067,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2082,10 +2082,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2132,7 +2132,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -2155,11 +2155,11 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -2221,10 +2221,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2260,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2275,10 +2275,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -2348,10 +2348,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -2413,10 +2413,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2452,7 +2452,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2467,10 +2467,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -2605,10 +2605,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>41</v>
@@ -2644,7 +2644,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2659,10 +2659,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -2732,14 +2732,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -2800,10 +2800,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>43</v>
@@ -2839,7 +2839,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2854,10 +2854,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2904,7 +2904,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -2927,10 +2927,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -2944,11 +2944,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -3009,10 +3009,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3048,7 +3048,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3063,10 +3063,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -3136,13 +3136,13 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -3189,7 +3189,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3329,10 +3329,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3368,7 +3368,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3383,10 +3383,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -3456,10 +3456,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="15"/>
@@ -3474,10 +3474,10 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -3539,10 +3539,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3578,7 +3578,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3593,10 +3593,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -3666,10 +3666,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -3685,11 +3685,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -3750,10 +3750,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3768,7 +3768,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -3789,7 +3789,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3804,10 +3804,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3854,7 +3854,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -3877,14 +3877,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -3898,11 +3898,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -3963,10 +3963,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>57</v>
@@ -4002,7 +4002,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -4017,10 +4017,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -4067,7 +4067,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -4090,10 +4090,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -4109,11 +4109,11 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -4128,10 +4128,10 @@
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4181,10 +4181,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -4199,7 +4199,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -4220,7 +4220,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -4235,10 +4235,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -4308,14 +4308,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="20"/>
@@ -4392,10 +4392,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -4431,7 +4431,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -4446,10 +4446,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -4496,7 +4496,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -4519,14 +4519,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -4540,10 +4540,10 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="16"/>
@@ -4607,10 +4607,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -4646,7 +4646,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -4661,10 +4661,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -4723,7 +4723,7 @@
         <v>78</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -4736,17 +4736,17 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -4806,10 +4806,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -4824,7 +4824,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -4860,10 +4860,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -4910,7 +4910,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -4933,10 +4933,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -4999,10 +4999,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -5053,10 +5053,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -5103,7 +5103,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -5126,10 +5126,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -5192,10 +5192,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -5210,7 +5210,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -5246,10 +5246,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -5319,10 +5319,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -5364,14 +5364,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5380,8 +5380,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="7" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="8" style="0" width="8.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -5394,8 +5394,9 @@
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -5414,10 +5415,13 @@
       <c r="F2" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>69</v>
@@ -5429,7 +5433,7 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>69</v>
@@ -5441,7 +5445,7 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>69</v>
@@ -5453,7 +5457,7 @@
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>69</v>
@@ -5465,7 +5469,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5503,10 +5507,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -5521,7 +5525,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -5557,10 +5561,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -5607,7 +5611,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -5630,14 +5634,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -5680,12 +5684,12 @@
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5698,10 +5702,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -5716,7 +5720,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>59</v>
@@ -5752,10 +5756,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -5802,7 +5806,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -5825,14 +5829,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
@@ -5879,7 +5883,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N12" activeCellId="0" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5922,28 +5926,28 @@
         <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>76</v>
@@ -5954,13 +5958,15 @@
       <c r="L2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -5979,7 +5985,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -5998,7 +6004,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -6017,7 +6023,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -6035,9 +6041,8 @@
       <c r="O6" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
+  <mergeCells count="1">
+    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6056,12 +6061,12 @@
   </sheetPr>
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="T12" activeCellId="0" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6095,70 +6100,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>62</v>
@@ -6167,19 +6172,19 @@
         <v>63</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -6205,14 +6210,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -6238,14 +6243,14 @@
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -6271,14 +6276,14 @@
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -6304,14 +6309,14 @@
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -6337,7 +6342,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -6359,7 +6364,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="6"/>
@@ -6370,18 +6375,18 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>69</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -6403,7 +6408,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="6"/>
@@ -6414,7 +6419,7 @@
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -6437,7 +6442,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="U10" s="6"/>
       <c r="V10" s="2"/>
@@ -6447,7 +6452,7 @@
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -6470,7 +6475,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="U11" s="6"/>
       <c r="V11" s="2"/>
@@ -6480,7 +6485,7 @@
     </row>
     <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -6503,7 +6508,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="U12" s="6"/>
       <c r="V12" s="2"/>
@@ -7979,10 +7984,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -7997,7 +8002,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>33</v>
@@ -8018,7 +8023,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -8033,10 +8038,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -8083,7 +8088,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -8106,10 +8111,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -8172,10 +8177,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -8190,7 +8195,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>33</v>
@@ -8211,7 +8216,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -8226,10 +8231,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -8276,7 +8281,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>76</v>
@@ -8299,11 +8304,11 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
@@ -8365,10 +8370,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -8383,7 +8388,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>37</v>
@@ -8404,7 +8409,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -8419,10 +8424,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -8469,7 +8474,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -8492,10 +8497,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -8558,10 +8563,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -8576,7 +8581,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>37</v>
@@ -8597,7 +8602,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -8612,10 +8617,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -8662,7 +8667,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
@@ -8685,10 +8690,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>

</xml_diff>

<commit_message>
Fix typos in constraint names
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
     <sheet name="Speaker conflict" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Talk mutually-exclusive-talks tags" sheetId="19" state="visible" r:id="rId20"/>
     <sheet name="Talk mutually-exclusive-talks tags 2" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="Talk mutually-exclusive-talks tag 3" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Talk mutually-exclusive-talks tags 3" sheetId="21" state="visible" r:id="rId22"/>
     <sheet name="Talk mutually-exclusive-talks tags 4" sheetId="22" state="visible" r:id="rId23"/>
     <sheet name="Talk mutually-exclusive-talks tags 5" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="Talk prerequisite talks" sheetId="24" state="visible" r:id="rId25"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="198">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -629,12 +629,6 @@
   </si>
   <si>
     <t xml:space="preserve">Speaker has conflicting timeslots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talk mutually-exclusive-talks tag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s</t>
   </si>
   <si>
     <t xml:space="preserve">Mutually exclusive talks in non-overlapping timeslots</t>
@@ -3393,7 +3387,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3427,10 +3421,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -3448,7 +3439,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3757,7 +3748,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3791,10 +3782,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -3812,7 +3800,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4004,10 +3992,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -4025,7 +4010,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4184,7 +4169,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4218,10 +4203,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -4239,7 +4221,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4257,7 +4239,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -4395,12 +4377,12 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4434,10 +4416,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -4455,7 +4434,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4473,7 +4452,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -4616,7 +4595,7 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -4673,7 +4652,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4884,7 +4863,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5099,7 +5078,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5298,7 +5277,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5491,7 +5470,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5509,7 +5488,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5684,7 +5663,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6058,7 +6037,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6253,7 +6232,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6448,7 +6427,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6643,7 +6622,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6842,7 +6821,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6860,7 +6839,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7041,7 +7020,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7059,7 +7038,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7240,7 +7219,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7258,7 +7237,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7439,7 +7418,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7457,7 +7436,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7640,7 +7619,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7658,7 +7637,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7858,7 +7837,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7876,7 +7855,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8273,7 +8252,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8291,7 +8270,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8491,7 +8470,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8509,7 +8488,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8709,7 +8688,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8727,7 +8706,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8932,7 +8911,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8950,7 +8929,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9155,7 +9134,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9173,7 +9152,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9374,7 +9353,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9392,7 +9371,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9597,7 +9576,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9615,7 +9594,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>

</xml_diff>

<commit_message>
Fix typo in test xlsx file
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="197">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Talk mutually-exclusive-talks tags</t>
   </si>
   <si>
-    <t xml:space="preserve">Hard penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>
+    <t xml:space="preserve">Medium penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>
   </si>
   <si>
     <t xml:space="preserve">Talk type of timeslot</t>
@@ -541,65 +541,12 @@
     <t xml:space="preserve">Timeslot with non matching talk type</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-1hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/0medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/0soft</t>
-    </r>
+    <t xml:space="preserve">-1hard/0medium/0soft</t>
   </si>
   <si>
     <t xml:space="preserve">Talk with available room</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">0hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/0medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/0soft</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Talk with unavailable room</t>
   </si>
   <si>
@@ -630,32 +577,7 @@
     <t xml:space="preserve">Mutually exclusive talks in non-overlapping timeslots</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">0hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/0medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/-1soft</t>
-    </r>
+    <t xml:space="preserve">0hard/0medium/-1soft</t>
   </si>
   <si>
     <t xml:space="preserve">Not Mutually exclusive talks in overlapping timeslots</t>
@@ -664,60 +586,10 @@
     <t xml:space="preserve">Mutually exclusive talks in overlapping timeslots</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">0hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/-1medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/-1soft</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">0hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/-2medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/-3soft</t>
-    </r>
+    <t xml:space="preserve">0hard/-1medium/-1soft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0hard/-2medium/-3soft</t>
   </si>
   <si>
     <t xml:space="preserve">Three Mutually exclusive talks in overlapping timeslots</t>
@@ -732,32 +604,7 @@
     <t xml:space="preserve">Talk scheduled before its prerequisites</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-2hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/0medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/0soft</t>
-    </r>
+    <t xml:space="preserve">-2hard/0medium/0soft</t>
   </si>
   <si>
     <t xml:space="preserve">Two talks with common theme and content tags on the same day</t>
@@ -775,32 +622,7 @@
     <t xml:space="preserve">Two talks with same content and same theme tags on different days</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">0hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/0medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/-2soft</t>
-    </r>
+    <t xml:space="preserve">0hard/0medium/-2soft</t>
   </si>
   <si>
     <t xml:space="preserve">Talks with different popularity in same room</t>
@@ -818,32 +640,7 @@
     <t xml:space="preserve">Three less popular talk in a bigger room than a more popular talk</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">0hard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">/0medium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/-3soft</t>
-    </r>
+    <t xml:space="preserve">0hard/0medium/-3soft</t>
   </si>
   <si>
     <t xml:space="preserve">Single normal talk and a pair of talks with greater than zero crowd control risk</t>
@@ -869,7 +666,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -903,11 +700,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1129,11 +921,11 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1626,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1644,7 +1436,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1821,7 +1613,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2015,7 +1807,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2033,7 +1825,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -2224,7 +2016,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2242,7 +2034,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -2416,7 +2208,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2434,7 +2226,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -2609,7 +2401,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2801,7 +2593,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2993,7 +2785,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3011,7 +2803,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -3188,7 +2980,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3397,7 +3189,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3415,7 +3207,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -3758,7 +3550,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3776,7 +3568,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -3968,7 +3760,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3986,7 +3778,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -4179,7 +3971,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4197,7 +3989,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -4392,7 +4184,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4410,7 +4202,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -4610,7 +4402,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4821,7 +4613,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4839,7 +4631,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5036,7 +4828,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5054,7 +4846,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5235,7 +5027,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5428,7 +5220,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5446,7 +5238,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5621,7 +5413,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5995,7 +5787,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6190,7 +5982,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6385,7 +6177,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6403,7 +6195,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -6580,7 +6372,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6598,7 +6390,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -6779,7 +6571,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6797,7 +6589,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -6978,7 +6770,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6996,7 +6788,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7177,7 +6969,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7195,7 +6987,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7376,7 +7168,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7394,7 +7186,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7577,7 +7369,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7595,7 +7387,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7795,7 +7587,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7813,7 +7605,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8210,7 +8002,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8228,7 +8020,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8428,7 +8220,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8446,7 +8238,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8646,7 +8438,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8664,7 +8456,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8869,7 +8661,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8887,7 +8679,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9092,7 +8884,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9110,7 +8902,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9311,7 +9103,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9329,7 +9121,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9534,7 +9326,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9552,7 +9344,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -12254,7 +12046,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -12429,7 +12221,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>

</xml_diff>

<commit_message>
Fix broken conf scheduling scoreRules test
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="21"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,42 +33,37 @@
     <sheet name="Talk prerequisite talks" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="Talk prerequisite talks 2" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="Talk prerequisite talks 3" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="Talk prerequisite talks 4" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="Talk prerequisite talks 5" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="Talk prerequisite talks 6" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="Talk prerequisite talks 7" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="Talk prerequisite talks 8" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="Same day talks 1" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="Same day talks 2" sheetId="32" state="visible" r:id="rId33"/>
-    <sheet name="Same day talks 3" sheetId="33" state="visible" r:id="rId34"/>
-    <sheet name="Same day talks 4" sheetId="34" state="visible" r:id="rId35"/>
-    <sheet name="Same day talks 5" sheetId="35" state="visible" r:id="rId36"/>
-    <sheet name="Popular talks 1" sheetId="36" state="visible" r:id="rId37"/>
-    <sheet name="Popular talks 2" sheetId="37" state="visible" r:id="rId38"/>
-    <sheet name="Popular talks 3" sheetId="38" state="visible" r:id="rId39"/>
-    <sheet name="Popular talks 4" sheetId="39" state="visible" r:id="rId40"/>
-    <sheet name="Popular talks 5" sheetId="40" state="visible" r:id="rId41"/>
-    <sheet name="Crowd control" sheetId="41" state="visible" r:id="rId42"/>
-    <sheet name="Crowd control 2" sheetId="42" state="visible" r:id="rId43"/>
-    <sheet name="Crowd control 3" sheetId="43" state="visible" r:id="rId44"/>
-    <sheet name="Crowd control 4" sheetId="44" state="visible" r:id="rId45"/>
-    <sheet name="Crowd control 5" sheetId="45" state="visible" r:id="rId46"/>
-    <sheet name="Published timeslot 1" sheetId="46" state="visible" r:id="rId47"/>
-    <sheet name="Published timeslot 2" sheetId="47" state="visible" r:id="rId48"/>
-    <sheet name="Published timeslot 3" sheetId="48" state="visible" r:id="rId49"/>
-    <sheet name="Published room 1" sheetId="49" state="visible" r:id="rId50"/>
-    <sheet name="Published room 2" sheetId="50" state="visible" r:id="rId51"/>
-    <sheet name="Published room 3" sheetId="51" state="visible" r:id="rId52"/>
-    <sheet name="Room stability 1" sheetId="52" state="visible" r:id="rId53"/>
-    <sheet name="Room stability 2" sheetId="53" state="visible" r:id="rId54"/>
-    <sheet name="Room stability 3" sheetId="54" state="visible" r:id="rId55"/>
-    <sheet name="Room stability 4" sheetId="55" state="visible" r:id="rId56"/>
-    <sheet name="Room stability 5" sheetId="56" state="visible" r:id="rId57"/>
-    <sheet name="Consecutive talks pause 1" sheetId="57" state="visible" r:id="rId58"/>
-    <sheet name="Consecutive talks pause 2" sheetId="58" state="visible" r:id="rId59"/>
-    <sheet name="Consecutive talks pause 3" sheetId="59" state="visible" r:id="rId60"/>
-    <sheet name="Consecutive talks pause 4" sheetId="60" state="visible" r:id="rId61"/>
-    <sheet name="Consecutive talks pause 5" sheetId="61" state="visible" r:id="rId62"/>
+    <sheet name="Same day talks 1" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="Same day talks 2" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="Same day talks 3" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="Same day talks 4" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="Same day talks 5" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="Popular talks 1" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="Popular talks 2" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="Popular talks 3" sheetId="33" state="visible" r:id="rId34"/>
+    <sheet name="Popular talks 4" sheetId="34" state="visible" r:id="rId35"/>
+    <sheet name="Popular talks 5" sheetId="35" state="visible" r:id="rId36"/>
+    <sheet name="Crowd control" sheetId="36" state="visible" r:id="rId37"/>
+    <sheet name="Crowd control 2" sheetId="37" state="visible" r:id="rId38"/>
+    <sheet name="Crowd control 3" sheetId="38" state="visible" r:id="rId39"/>
+    <sheet name="Crowd control 4" sheetId="39" state="visible" r:id="rId40"/>
+    <sheet name="Crowd control 5" sheetId="40" state="visible" r:id="rId41"/>
+    <sheet name="Published timeslot 1" sheetId="41" state="visible" r:id="rId42"/>
+    <sheet name="Published timeslot 2" sheetId="42" state="visible" r:id="rId43"/>
+    <sheet name="Published timeslot 3" sheetId="43" state="visible" r:id="rId44"/>
+    <sheet name="Published room 1" sheetId="44" state="visible" r:id="rId45"/>
+    <sheet name="Published room 2" sheetId="45" state="visible" r:id="rId46"/>
+    <sheet name="Published room 3" sheetId="46" state="visible" r:id="rId47"/>
+    <sheet name="Room stability 1" sheetId="47" state="visible" r:id="rId48"/>
+    <sheet name="Room stability 2" sheetId="48" state="visible" r:id="rId49"/>
+    <sheet name="Room stability 3" sheetId="49" state="visible" r:id="rId50"/>
+    <sheet name="Room stability 4" sheetId="50" state="visible" r:id="rId51"/>
+    <sheet name="Room stability 5" sheetId="51" state="visible" r:id="rId52"/>
+    <sheet name="Consecutive talks pause 1" sheetId="52" state="visible" r:id="rId53"/>
+    <sheet name="Consecutive talks pause 2" sheetId="53" state="visible" r:id="rId54"/>
+    <sheet name="Consecutive talks pause 3" sheetId="54" state="visible" r:id="rId55"/>
+    <sheet name="Consecutive talks pause 4" sheetId="55" state="visible" r:id="rId56"/>
+    <sheet name="Consecutive talks pause 5" sheetId="56" state="visible" r:id="rId57"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -80,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="230">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -665,9 +660,6 @@
   </si>
   <si>
     <t xml:space="preserve">Talk scheduled after its prerequisites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talk scheduled before its prerequisites</t>
   </si>
   <si>
     <t xml:space="preserve">Two talks with common theme and content tags on the same day</t>
@@ -4106,12 +4098,10 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4949,7 +4939,7 @@
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -4988,7 +4978,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -5024,7 +5014,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5097,10 +5087,12 @@
         <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
+      <c r="D8" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -5181,7 +5173,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -5199,7 +5191,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5217,7 +5209,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5252,7 +5244,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -5275,7 +5269,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -5290,11 +5286,13 @@
         <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -5374,7 +5372,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -5392,7 +5390,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5410,7 +5408,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5445,7 +5443,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -5468,7 +5468,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -5483,11 +5485,13 @@
         <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -5567,7 +5571,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -5585,7 +5589,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5603,7 +5607,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5638,7 +5642,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -5661,7 +5667,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -5676,13 +5684,13 @@
         <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" s="15"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -5951,7 +5959,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -5969,7 +5977,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5987,7 +5995,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -6022,7 +6030,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -6045,7 +6055,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -6060,13 +6072,13 @@
         <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" s="15"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -6117,7 +6129,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
@@ -6146,7 +6158,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -6164,7 +6176,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6217,7 +6229,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -6240,7 +6254,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -6251,17 +6267,19 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
+      <c r="A8" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="15"/>
+        <v>164</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>165</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -6300,7 +6318,7 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -6312,7 +6330,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
@@ -6341,7 +6359,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -6359,7 +6377,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6412,9 +6430,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -6437,9 +6453,7 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -6450,17 +6464,15 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
+      <c r="A8" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>152</v>
-      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -6470,8 +6482,33 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6499,7 +6536,7 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -6511,7 +6548,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
@@ -6540,7 +6577,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -6558,7 +6595,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6576,7 +6613,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -6611,9 +6648,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -6636,9 +6671,7 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -6649,17 +6682,15 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
+      <c r="A8" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>157</v>
-      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -6669,8 +6700,33 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6698,7 +6754,7 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -6710,7 +6766,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
@@ -6739,7 +6795,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -6757,7 +6813,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6775,7 +6831,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -6810,9 +6866,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -6835,9 +6889,7 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -6848,17 +6900,15 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
+      <c r="A8" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -6868,8 +6918,33 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6897,7 +6972,7 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -6909,7 +6984,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
@@ -6938,7 +7013,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -6956,7 +7031,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6974,7 +7049,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7009,9 +7084,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -7034,9 +7107,7 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -7047,17 +7118,15 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
+      <c r="A8" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -7067,8 +7136,33 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7096,7 +7190,7 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -7137,7 +7231,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -7155,7 +7249,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7246,19 +7340,17 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>162</v>
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>165</v>
-      </c>
+      <c r="D8" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -7268,8 +7360,32 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="0"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+    </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7338,7 +7454,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -7356,7 +7472,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7374,7 +7490,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7409,7 +7525,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -7432,7 +7550,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -7443,15 +7563,15 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>162</v>
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -7462,13 +7582,13 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="0"/>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
@@ -7481,12 +7601,13 @@
       <c r="M9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>165</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7556,7 +7677,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -7574,7 +7695,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7592,7 +7713,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7627,7 +7748,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -7650,7 +7773,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -7661,15 +7786,15 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>164</v>
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -7680,13 +7805,11 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
@@ -7699,12 +7822,11 @@
       <c r="M9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>165</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7774,7 +7896,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -7792,7 +7914,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -7810,7 +7932,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -7845,7 +7967,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -7868,7 +7992,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -7879,15 +8005,19 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>164</v>
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>168</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -7898,14 +8028,12 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="0"/>
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -7917,12 +8045,11 @@
       <c r="M9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8160,7 +8287,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8194,7 +8321,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -8212,7 +8339,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8230,7 +8357,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8265,7 +8392,9 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -8288,7 +8417,9 @@
       <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -8299,15 +8430,17 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>165</v>
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="0" t="s">
+        <v>168</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -8318,15 +8451,17 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="15"/>
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="0" t="s">
+        <v>169</v>
+      </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="15"/>
@@ -8337,12 +8472,13 @@
       <c r="M9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8371,14 +8507,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8412,7 +8548,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -8430,7 +8566,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8521,16 +8657,12 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>166</v>
-      </c>
+      <c r="A8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="0"/>
       <c r="C8" s="0"/>
-      <c r="D8" s="0" t="s">
-        <v>142</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -8543,14 +8675,14 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>167</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B9" s="0"/>
       <c r="C9" s="0"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="0"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="15"/>
@@ -8560,13 +8692,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8594,14 +8720,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8635,7 +8761,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -8653,7 +8779,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8671,7 +8797,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8745,10 +8871,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>166</v>
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -8764,14 +8890,12 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>167</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B9" s="0"/>
       <c r="C9" s="0"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="15"/>
@@ -8781,15 +8905,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="0"/>
-    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8817,14 +8933,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8858,7 +8974,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -8876,7 +8992,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -8894,7 +9010,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -8968,13 +9084,13 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>166</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B8" s="0"/>
       <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
+      <c r="D8" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -8987,12 +9103,12 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="15"/>
@@ -9002,13 +9118,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9036,14 +9146,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9077,7 +9187,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -9095,7 +9205,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9113,7 +9223,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9186,19 +9296,13 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>166</v>
-      </c>
+      <c r="A8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="0"/>
       <c r="C8" s="0"/>
-      <c r="D8" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>168</v>
-      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -9210,12 +9314,14 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="0"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="15"/>
@@ -9225,13 +9331,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9259,14 +9359,14 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9300,7 +9400,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -9318,7 +9418,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9410,16 +9510,14 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>166</v>
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
-      <c r="E8" s="0" t="s">
-        <v>168</v>
-      </c>
+      <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="15"/>
@@ -9431,16 +9529,12 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0"/>
-      <c r="C9" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="0" t="s">
-        <v>169</v>
-      </c>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="15"/>
@@ -9450,15 +9544,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="0"/>
-    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9493,7 +9579,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9527,7 +9613,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -9545,7 +9631,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9563,7 +9649,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -9636,12 +9722,12 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="0"/>
       <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -9656,11 +9742,11 @@
       <c r="A9" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="C9" s="0"/>
-      <c r="D9" s="0" t="s">
-        <v>142</v>
-      </c>
+      <c r="D9" s="0"/>
       <c r="E9" s="0"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -9706,7 +9792,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9740,7 +9826,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -9758,7 +9844,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9850,13 +9936,15 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>170</v>
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
+      <c r="D8" s="0" t="s">
+        <v>145</v>
+      </c>
       <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -9869,9 +9957,9 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="0"/>
+        <v>102</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="0"/>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
@@ -9919,7 +10007,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9953,7 +10041,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -9971,7 +10059,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -9989,7 +10077,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -10063,13 +10151,13 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="0"/>
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>142</v>
+      </c>
       <c r="C8" s="0"/>
-      <c r="D8" s="2" t="s">
-        <v>170</v>
-      </c>
+      <c r="D8" s="0"/>
       <c r="E8" s="0"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -10082,11 +10170,13 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="0"/>
+        <v>102</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
+      <c r="D9" s="0" t="s">
+        <v>145</v>
+      </c>
       <c r="E9" s="0"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -10132,7 +10222,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10166,7 +10256,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -10184,7 +10274,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -10275,10 +10365,12 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="0"/>
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>142</v>
+      </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
@@ -10293,14 +10385,14 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="0"/>
+        <v>102</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="0"/>
-      <c r="D9" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0" t="s">
+        <v>145</v>
+      </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="15"/>
@@ -12478,7 +12570,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12512,7 +12604,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -12530,7 +12622,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -12622,10 +12714,10 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>170</v>
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -12641,10 +12733,12 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
+        <v>102</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="0" t="s">
+        <v>152</v>
+      </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
       <c r="F9" s="16"/>
@@ -12684,7 +12778,7 @@
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -12725,7 +12819,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -12743,7 +12837,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -12761,7 +12855,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -12835,9 +12929,11 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="0"/>
+        <v>101</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
@@ -12852,10 +12948,10 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" s="0"/>
@@ -12869,7 +12965,15 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="0"/>
+    </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12892,1089 +12996,6 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="0"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:D6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E9" s="0"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:D6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:D6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:D6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="10" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:D6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
@@ -14043,7 +13064,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -14202,7 +13223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
@@ -14271,7 +13292,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -14413,7 +13434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
@@ -14482,7 +13503,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -14592,6 +13613,445 @@
       </c>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="10" width="19.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="10" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="10" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6"/>
+      <c r="B6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF00DCFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="10" width="19.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="10" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="10" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6"/>
+      <c r="B6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="16" t="s">
+        <v>145</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="15"/>
@@ -14817,445 +14277,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:N10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="10" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:E6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FF00DCFF"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:N9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="10" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="10" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:E6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">

</xml_diff>

<commit_message>
Fix style and typo in test file
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/solver/testConferenceSchedulingScoreRules.xlsx
@@ -231,7 +231,7 @@
     <t xml:space="preserve">Audience type theme track conflict</t>
   </si>
   <si>
-    <t xml:space="preserve">Penalty per 2 talks with a common audience type, a common theme track and overlapping timeslotst, per overlapping minute</t>
+    <t xml:space="preserve">Penalty per 2 talks with a common audience type, a common theme track and overlapping timeslots, per overlapping minute</t>
   </si>
   <si>
     <t xml:space="preserve">Audience level diversity</t>
@@ -980,7 +980,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>